<commit_message>
upload superived train 0.2k/0.4k/2k/5k
</commit_message>
<xml_diff>
--- a/res_img/resnet50-moreways-10k-size(768)-medium-trainset(1k)/动态.xlsx
+++ b/res_img/resnet50-moreways-10k-size(768)-medium-trainset(1k)/动态.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Remote_GDJC\res_img\resnet50-moreways-10k-size(768)-medium-trainset(1k)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B852AA78-BFA4-460A-87B4-1167F293035E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEDF38D-5331-4D39-B37D-61FE672940C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>map</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -104,10 +104,6 @@
     <t>15k</t>
   </si>
   <si>
-    <t>15k——&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>block</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -116,15 +112,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>moreways</t>
+    <t>3k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>anchor size</t>
+    <t>3 way</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0.23/0.22</t>
+    <t>more ways</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cutpaste methods</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1565,16 +1565,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>2722</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>672193</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>394607</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>146956</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>367393</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>87084</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1865,15 +1865,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1906,8 +1906,11 @@
       <c r="E2">
         <v>4.8000000000000001E-2</v>
       </c>
+      <c r="G2">
+        <v>0.27700000000000002</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1923,8 +1926,11 @@
       <c r="E3">
         <v>7.0000000000000007E-2</v>
       </c>
+      <c r="G3">
+        <v>0.39500000000000002</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1940,8 +1946,11 @@
       <c r="E4">
         <v>4.3999999999999997E-2</v>
       </c>
+      <c r="G4">
+        <v>0.38300000000000001</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1957,8 +1966,11 @@
       <c r="E5">
         <v>7.4999999999999997E-2</v>
       </c>
+      <c r="G5">
+        <v>0.47899999999999998</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1974,8 +1986,11 @@
       <c r="E6">
         <v>0.13500000000000001</v>
       </c>
+      <c r="G6">
+        <v>0.47399999999999998</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1991,8 +2006,11 @@
       <c r="E7">
         <v>0.157</v>
       </c>
+      <c r="G7">
+        <v>0.52700000000000002</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2008,8 +2026,11 @@
       <c r="E8">
         <v>9.9000000000000005E-2</v>
       </c>
+      <c r="G8">
+        <v>0.52700000000000002</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2025,8 +2046,11 @@
       <c r="E9">
         <v>0.121</v>
       </c>
+      <c r="G9">
+        <v>0.54900000000000004</v>
+      </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2042,8 +2066,11 @@
       <c r="E10">
         <v>0.14699999999999999</v>
       </c>
+      <c r="G10">
+        <v>0.53800000000000003</v>
+      </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2059,8 +2086,11 @@
       <c r="E11">
         <v>0.14799999999999999</v>
       </c>
+      <c r="G11">
+        <v>0.54700000000000004</v>
+      </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2076,8 +2106,11 @@
       <c r="E12">
         <v>0.11600000000000001</v>
       </c>
+      <c r="G12">
+        <v>0.55300000000000005</v>
+      </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2093,8 +2126,11 @@
       <c r="E13">
         <v>0.12</v>
       </c>
+      <c r="G13">
+        <v>0.55400000000000005</v>
+      </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2110,8 +2146,11 @@
       <c r="E14">
         <v>0.20100000000000001</v>
       </c>
+      <c r="G14">
+        <v>0.54600000000000004</v>
+      </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2127,8 +2166,11 @@
       <c r="E15">
         <v>0.20399999999999999</v>
       </c>
+      <c r="G15">
+        <v>0.57799999999999996</v>
+      </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -2144,8 +2186,11 @@
       <c r="E16">
         <v>0.16200000000000001</v>
       </c>
+      <c r="G16">
+        <v>0.57799999999999996</v>
+      </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B19">
         <f>SUM(B14:B16)/3</f>
         <v>0.60199999999999998</v>
@@ -2163,68 +2208,254 @@
         <v>0.18900000000000003</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
       <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" t="s">
+        <v>12</v>
+      </c>
+      <c r="J22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22" t="s">
+        <v>18</v>
+      </c>
+      <c r="P22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.317</v>
+      </c>
+      <c r="D23">
+        <v>0.42</v>
+      </c>
+      <c r="E23">
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="F23">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="H23">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="I23">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="J23">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="K23">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="L23">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="M23">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="N23">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="O23">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="P23">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>21</v>
       </c>
-      <c r="E22" t="s">
-        <v>5</v>
+      <c r="B24">
+        <v>0.27</v>
+      </c>
+      <c r="C24">
+        <v>0.28199999999999997</v>
+      </c>
+      <c r="D24">
+        <v>0.30199999999999999</v>
+      </c>
+      <c r="E24">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="F24">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="G24">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="H24">
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="I24">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="J24">
+        <v>0.42</v>
+      </c>
+      <c r="K24">
+        <v>0.46</v>
+      </c>
+      <c r="L24">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="M24">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="N24">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O24">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="P24">
+        <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>20</v>
       </c>
-      <c r="C24" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24">
-        <v>32</v>
-      </c>
-      <c r="F24">
-        <v>64</v>
-      </c>
-      <c r="G24">
-        <v>128</v>
-      </c>
-      <c r="H24">
-        <v>256</v>
-      </c>
-      <c r="I24">
-        <v>512</v>
-      </c>
-      <c r="K24">
-        <v>768</v>
+      <c r="B25">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C25">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="D25">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="E25">
+        <v>0.34</v>
+      </c>
+      <c r="F25">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="G25">
+        <v>0.37</v>
+      </c>
+      <c r="H25">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="I25">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="J25">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="K25">
+        <v>0.49</v>
+      </c>
+      <c r="L25">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="M25">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="N25">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="O25">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="P25">
+        <v>0.56599999999999995</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="H27">
-        <v>512</v>
-      </c>
-      <c r="I27">
-        <v>1024</v>
-      </c>
-      <c r="K27">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="C28" t="s">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="H29">
-        <v>10000</v>
-      </c>
-      <c r="I29">
-        <v>15000</v>
-      </c>
-      <c r="K29" t="s">
-        <v>25</v>
+      <c r="B26">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="C26">
+        <v>0.312</v>
+      </c>
+      <c r="D26">
+        <v>0.34</v>
+      </c>
+      <c r="E26">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="F26">
+        <v>0.35</v>
+      </c>
+      <c r="G26">
+        <v>0.42</v>
+      </c>
+      <c r="H26">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="I26">
+        <v>0.47</v>
+      </c>
+      <c r="J26">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="K26">
+        <v>0.52</v>
+      </c>
+      <c r="L26">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="M26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="N26">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="O26">
+        <v>0.56200000000000006</v>
+      </c>
+      <c r="P26">
+        <v>0.56000000000000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>